<commit_message>
settled on an opcode encoding
</commit_message>
<xml_diff>
--- a/cpu_design.xlsx
+++ b/cpu_design.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\stack-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF391C2-98B4-4D3A-9221-62CFFF0E935D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6BE7EC-7386-4815-A972-CCA2CF3CF852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="2220" windowWidth="27855" windowHeight="13980" xr2:uid="{91C87F09-169E-4D7F-9DD3-941A697827A4}"/>
+    <workbookView xWindow="945" yWindow="2220" windowWidth="27855" windowHeight="13980" firstSheet="1" activeTab="3" xr2:uid="{91C87F09-169E-4D7F-9DD3-941A697827A4}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
     <sheet name="memory" sheetId="2" r:id="rId2"/>
+    <sheet name="helper functions" sheetId="3" r:id="rId3"/>
+    <sheet name="addressing_modes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="108">
   <si>
     <t>arithmetic</t>
   </si>
@@ -157,9 +159,6 @@
     <t>sbb</t>
   </si>
   <si>
-    <t>hop</t>
-  </si>
-  <si>
     <t>call short</t>
   </si>
   <si>
@@ -175,9 +174,6 @@
     <t>more useful, 16 bit pc version</t>
   </si>
   <si>
-    <t>stripped down, 8 bit version</t>
-  </si>
-  <si>
     <t>right shift</t>
   </si>
   <si>
@@ -193,16 +189,178 @@
     <t>different encodings</t>
   </si>
   <si>
-    <t>adressing modes</t>
-  </si>
-  <si>
-    <t>2 operand math</t>
-  </si>
-  <si>
-    <t>vstack, rstack</t>
-  </si>
-  <si>
-    <t>vstack</t>
+    <t>jump short</t>
+  </si>
+  <si>
+    <t>add16 given two little endian integers</t>
+  </si>
+  <si>
+    <t>stack in</t>
+  </si>
+  <si>
+    <t>a_low</t>
+  </si>
+  <si>
+    <t>a_high</t>
+  </si>
+  <si>
+    <t>b_low</t>
+  </si>
+  <si>
+    <t>b_high</t>
+  </si>
+  <si>
+    <t>vtr</t>
+  </si>
+  <si>
+    <t>rtv</t>
+  </si>
+  <si>
+    <t>move val to ret</t>
+  </si>
+  <si>
+    <t>move ret to val</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>neg</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>imm</t>
+  </si>
+  <si>
+    <t>swp</t>
+  </si>
+  <si>
+    <t>bz</t>
+  </si>
+  <si>
+    <t>jmp</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>stripped down, 8 bit version, 4 bit instructions</t>
+  </si>
+  <si>
+    <t>slr</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t>2 operands</t>
+  </si>
+  <si>
+    <t>op0</t>
+  </si>
+  <si>
+    <t>op1</t>
+  </si>
+  <si>
+    <t>op2</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>both ret stack</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b0</t>
+  </si>
+  <si>
+    <t>mixed</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>can reach the most recent 4 values on the return stack for each argument</t>
+  </si>
+  <si>
+    <t>both val stack</t>
+  </si>
+  <si>
+    <t>args are two top values on val stack</t>
+  </si>
+  <si>
+    <t>1 operand</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>attempt 1</t>
+  </si>
+  <si>
+    <t>attempt 2</t>
+  </si>
+  <si>
+    <t>can reach the most recent 4 values on the return stack for second arg and top 2 for first</t>
+  </si>
+  <si>
+    <t>first arg is top of value stack, second one is one of last 4 values on return stack</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>first arg is top of value stack, second one is one of last 7 values on return stack</t>
+  </si>
+  <si>
+    <t>arg is one of 7 most recent values on ret stack</t>
+  </si>
+  <si>
+    <t>arg is top of the val stack</t>
+  </si>
+  <si>
+    <t>op3</t>
+  </si>
+  <si>
+    <t>1 num</t>
+  </si>
+  <si>
+    <t>ret stack</t>
+  </si>
+  <si>
+    <t>val stack</t>
+  </si>
+  <si>
+    <t>can reach the most recent 4 values on the return stack for either arg</t>
+  </si>
+  <si>
+    <t>0 operand</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>a2</t>
   </si>
 </sst>
 </file>
@@ -238,9 +396,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -557,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E14E15-FFEA-4089-8591-BA60CB9BCCD2}">
-  <dimension ref="A2:W46"/>
+  <dimension ref="B2:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +731,7 @@
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
     <col min="19" max="19" width="22.28515625" customWidth="1"/>
@@ -578,13 +739,13 @@
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="R2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
@@ -594,10 +755,10 @@
       <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>18</v>
       </c>
       <c r="T4" t="s">
@@ -609,40 +770,43 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
       <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
       <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" t="s">
         <v>43</v>
       </c>
-      <c r="M5" t="s">
-        <v>44</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="V5" t="s">
+        <v>42</v>
+      </c>
+      <c r="W5" t="s">
         <v>43</v>
-      </c>
-      <c r="O5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5" t="s">
-        <v>43</v>
-      </c>
-      <c r="W5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
@@ -670,16 +834,19 @@
       <c r="K6" t="s">
         <v>1</v>
       </c>
-      <c r="L6">
-        <v>2</v>
+      <c r="L6" t="s">
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>0</v>
       </c>
       <c r="R6" t="s">
@@ -720,20 +887,23 @@
       <c r="K7" t="s">
         <v>31</v>
       </c>
-      <c r="L7">
-        <v>1</v>
+      <c r="L7" t="s">
+        <v>62</v>
       </c>
       <c r="M7">
         <v>1</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
       <c r="S7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T7">
         <v>2</v>
@@ -765,22 +935,25 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
       <c r="S8" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="T8">
         <v>2</v>
@@ -812,22 +985,25 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
       <c r="S9" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="T9">
         <v>2</v>
@@ -859,22 +1035,25 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
       <c r="S10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="T10">
         <v>2</v>
@@ -906,25 +1085,28 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11">
-        <v>2</v>
+        <v>45</v>
+      </c>
+      <c r="L11" t="s">
+        <v>72</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
       <c r="S11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="T11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U11">
         <v>1</v>
@@ -953,25 +1135,28 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>73</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
       <c r="S12" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="T12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U12">
         <v>1</v>
@@ -1005,23 +1190,26 @@
       <c r="K13" t="s">
         <v>10</v>
       </c>
-      <c r="L13">
-        <v>0</v>
+      <c r="L13" t="s">
+        <v>64</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
       <c r="S13" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="T13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U13">
         <v>1</v>
@@ -1055,23 +1243,26 @@
       <c r="K14" t="s">
         <v>33</v>
       </c>
-      <c r="L14">
-        <v>1</v>
+      <c r="L14" t="s">
+        <v>33</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
       <c r="S14" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U14">
         <v>1</v>
@@ -1102,20 +1293,23 @@
       <c r="K15" t="s">
         <v>34</v>
       </c>
-      <c r="L15">
-        <v>2</v>
+      <c r="L15" t="s">
+        <v>65</v>
       </c>
       <c r="M15">
         <v>2</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
       <c r="S15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T15">
         <v>2</v>
@@ -1147,25 +1341,31 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>35</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="L16" t="s">
+        <v>57</v>
       </c>
       <c r="M16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>9</v>
       </c>
       <c r="S16" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="T16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16">
         <v>1</v>
@@ -1194,28 +1394,34 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>36</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="L17" t="s">
+        <v>58</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <v>1</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>32</v>
       </c>
       <c r="S17" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -1249,8 +1455,8 @@
       <c r="K18" t="s">
         <v>11</v>
       </c>
-      <c r="L18">
-        <v>0</v>
+      <c r="L18" t="s">
+        <v>66</v>
       </c>
       <c r="M18">
         <v>2</v>
@@ -1261,28 +1467,13 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="R18" t="s">
-        <v>9</v>
-      </c>
-      <c r="S18" t="s">
-        <v>10</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
+      <c r="P18">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1299,11 +1490,11 @@
       <c r="K19" t="s">
         <v>12</v>
       </c>
-      <c r="L19">
-        <v>1</v>
+      <c r="L19" t="s">
+        <v>67</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -1311,20 +1502,23 @@
       <c r="O19">
         <v>0</v>
       </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
       <c r="S19" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V19">
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
@@ -1349,32 +1543,32 @@
       <c r="K20" t="s">
         <v>29</v>
       </c>
-      <c r="L20">
-        <v>1</v>
+      <c r="L20" t="s">
+        <v>63</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="R20" t="s">
-        <v>32</v>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
       </c>
       <c r="S20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -1397,34 +1591,25 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" t="s">
         <v>28</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
         <v>0</v>
       </c>
       <c r="S21" t="s">
-        <v>34</v>
-      </c>
-      <c r="T21">
-        <v>2</v>
-      </c>
-      <c r="U21">
-        <v>2</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
@@ -1443,21 +1628,6 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="S22" t="s">
-        <v>35</v>
-      </c>
-      <c r="T22">
-        <v>1</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
@@ -1475,17 +1645,20 @@
       <c r="G23">
         <v>0</v>
       </c>
+      <c r="R23" t="s">
+        <v>5</v>
+      </c>
       <c r="S23" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23">
         <v>1</v>
       </c>
       <c r="V23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -1493,18 +1666,27 @@
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S24" t="s">
-        <v>49</v>
+        <v>7</v>
+      </c>
+      <c r="T24">
+        <v>2</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="S25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
@@ -1526,24 +1708,6 @@
       <c r="G26">
         <v>0</v>
       </c>
-      <c r="R26" t="s">
-        <v>5</v>
-      </c>
-      <c r="S26" t="s">
-        <v>6</v>
-      </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26">
-        <v>1</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
@@ -1561,19 +1725,56 @@
       <c r="G27">
         <v>0</v>
       </c>
+      <c r="R27" t="s">
+        <v>8</v>
+      </c>
       <c r="S27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="T27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V27">
         <v>0</v>
       </c>
       <c r="W27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="S28" t="s">
+        <v>12</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>2</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="S29" t="s">
+        <v>29</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="V29">
+        <v>2</v>
+      </c>
+      <c r="W29">
         <v>0</v>
       </c>
     </row>
@@ -1596,93 +1797,60 @@
       <c r="G30">
         <v>0</v>
       </c>
-      <c r="R30" t="s">
-        <v>8</v>
-      </c>
       <c r="S30" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="T30">
         <v>0</v>
       </c>
       <c r="U30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V30">
         <v>0</v>
       </c>
       <c r="W30">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>40</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="S32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T32">
-        <v>1</v>
-      </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
-      <c r="V32">
-        <v>0</v>
-      </c>
-      <c r="W32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>41</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="S33" t="s">
-        <v>41</v>
-      </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
-      <c r="U33">
-        <v>0</v>
-      </c>
-      <c r="V33">
-        <v>0</v>
-      </c>
-      <c r="W33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>42</v>
-      </c>
       <c r="D34">
         <v>0</v>
       </c>
@@ -1695,23 +1863,8 @@
       <c r="G34">
         <v>0</v>
       </c>
-      <c r="S34" t="s">
-        <v>42</v>
-      </c>
-      <c r="T34">
-        <v>0</v>
-      </c>
-      <c r="U34">
-        <v>0</v>
-      </c>
-      <c r="V34">
-        <v>1</v>
-      </c>
-      <c r="W34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>12</v>
       </c>
@@ -1727,23 +1880,8 @@
       <c r="G35">
         <v>0</v>
       </c>
-      <c r="S35" t="s">
-        <v>12</v>
-      </c>
-      <c r="T35">
-        <v>0</v>
-      </c>
-      <c r="U35">
-        <v>2</v>
-      </c>
-      <c r="V35">
-        <v>0</v>
-      </c>
-      <c r="W35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>29</v>
       </c>
@@ -1759,23 +1897,8 @@
       <c r="G36">
         <v>0</v>
       </c>
-      <c r="S36" t="s">
-        <v>29</v>
-      </c>
-      <c r="T36">
-        <v>0</v>
-      </c>
-      <c r="U36">
-        <v>2</v>
-      </c>
-      <c r="V36">
-        <v>2</v>
-      </c>
-      <c r="W36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>28</v>
       </c>
@@ -1790,50 +1913,6 @@
       </c>
       <c r="G37">
         <v>2</v>
-      </c>
-      <c r="S37" t="s">
-        <v>28</v>
-      </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
-      <c r="V37">
-        <v>0</v>
-      </c>
-      <c r="W37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>2</v>
-      </c>
-      <c r="B46" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1931,4 +2010,1365 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5328BF-A4A4-471E-8C93-D0D6477E0A93}">
+  <dimension ref="B3:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537D18CE-A36A-42D4-BC2F-69AB3A8EDA46}">
+  <dimension ref="B2:K77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="1">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1">
+        <v>5</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>3</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="1">
+        <v>7</v>
+      </c>
+      <c r="D36" s="1">
+        <v>6</v>
+      </c>
+      <c r="E36" s="1">
+        <v>5</v>
+      </c>
+      <c r="F36" s="1">
+        <v>4</v>
+      </c>
+      <c r="G36" s="1">
+        <v>3</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="1">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1">
+        <v>6</v>
+      </c>
+      <c r="E41" s="1">
+        <v>5</v>
+      </c>
+      <c r="F41" s="1">
+        <v>4</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3</v>
+      </c>
+      <c r="H41" s="1">
+        <v>2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="1">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1">
+        <v>6</v>
+      </c>
+      <c r="E45" s="1">
+        <v>5</v>
+      </c>
+      <c r="F45" s="1">
+        <v>4</v>
+      </c>
+      <c r="G45" s="1">
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>2</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>1</v>
+      </c>
+      <c r="J46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="1">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1">
+        <v>6</v>
+      </c>
+      <c r="E61" s="1">
+        <v>5</v>
+      </c>
+      <c r="F61" s="1">
+        <v>4</v>
+      </c>
+      <c r="G61" s="1">
+        <v>3</v>
+      </c>
+      <c r="H61" s="1">
+        <v>2</v>
+      </c>
+      <c r="I61" s="1">
+        <v>1</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0</v>
+      </c>
+      <c r="K61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0</v>
+      </c>
+      <c r="K62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J63" s="1">
+        <v>1</v>
+      </c>
+      <c r="K63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1">
+        <v>1</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+      <c r="K64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="1">
+        <v>7</v>
+      </c>
+      <c r="D67" s="1">
+        <v>6</v>
+      </c>
+      <c r="E67" s="1">
+        <v>5</v>
+      </c>
+      <c r="F67" s="1">
+        <v>4</v>
+      </c>
+      <c r="G67" s="1">
+        <v>3</v>
+      </c>
+      <c r="H67" s="1">
+        <v>2</v>
+      </c>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0</v>
+      </c>
+      <c r="K67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C68" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J68" s="1">
+        <v>1</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J69" s="1">
+        <v>1</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" s="1">
+        <v>7</v>
+      </c>
+      <c r="D72" s="1">
+        <v>6</v>
+      </c>
+      <c r="E72" s="1">
+        <v>5</v>
+      </c>
+      <c r="F72" s="1">
+        <v>4</v>
+      </c>
+      <c r="G72" s="1">
+        <v>3</v>
+      </c>
+      <c r="H72" s="1">
+        <v>2</v>
+      </c>
+      <c r="I72" s="1">
+        <v>1</v>
+      </c>
+      <c r="J72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" t="s">
+        <v>95</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>104</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C76" s="1">
+        <v>7</v>
+      </c>
+      <c r="D76" s="1">
+        <v>6</v>
+      </c>
+      <c r="E76" s="1">
+        <v>5</v>
+      </c>
+      <c r="F76" s="1">
+        <v>4</v>
+      </c>
+      <c r="G76" s="1">
+        <v>3</v>
+      </c>
+      <c r="H76" s="1">
+        <v>2</v>
+      </c>
+      <c r="I76" s="1">
+        <v>1</v>
+      </c>
+      <c r="J76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
+        <v>1</v>
+      </c>
+      <c r="H77" s="1">
+        <v>1</v>
+      </c>
+      <c r="I77" s="1">
+        <v>1</v>
+      </c>
+      <c r="J77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>